<commit_message>
Changes after executing Scheduler and Single execution agentic process for all the list
</commit_message>
<xml_diff>
--- a/src/data/output/Capgemini_Server_Data_Deviation_Analysis.xlsx
+++ b/src/data/output/Capgemini_Server_Data_Deviation_Analysis.xlsx
@@ -1666,7 +1666,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-02-04 21:22:57</t>
+          <t>2026-02-05 12:22:40</t>
         </is>
       </c>
     </row>
@@ -1749,10 +1749,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{0ffa499d-8334-4b45-bbba-5ec17299202b}" enabled="1" method="Privileged" siteId="{76a2ae5a-9f00-4f6b-95ed-5d33d77c4d61}" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>